<commit_message>
adding part of codes to the dataset
</commit_message>
<xml_diff>
--- a/Data/countries.xlsx
+++ b/Data/countries.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mr-Khosravian\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AlMetric-Research-Paper\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -95,36 +95,15 @@
     <t>japan; usa; uk; malysia; spain; canada; australia; germany; iran; switzerland</t>
   </si>
   <si>
-    <t xml:space="preserve">usa; uk; australia; italy; costa rica; germany; greece; ireland; mexico; new zealand; sweden; </t>
-  </si>
-  <si>
-    <t>usa; uk; india; australia; france; bangladesh; brazil; germany; philipines; new zealand; russia; canada; israel; italy; japan; malysia; netherlands; signapor; south africa; ukraine; uae; armenia; belgium; croatia; estonia; ireland; jamaica; jordan; nepal; nigeria; portugal; sweden; switzerland; turkey</t>
-  </si>
-  <si>
     <t>switzerland; france; belgium; uk; canada; Denmark; luxembourg; philipines; usa</t>
   </si>
   <si>
     <t>usa; uk; canada; france; spain; brazil; japan; germany; india; iran</t>
   </si>
   <si>
-    <t xml:space="preserve">usa; uk; canada; brazil; italy; india; australia; spain; norway; serbia; thailand; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">usa; uk; australia; india; germany; spain; canada; russia; france; italy; iran; </t>
-  </si>
-  <si>
-    <t>switzerland; usa; italy; philipines; uk; luxembourg; kenya; sweden; canada; netherlands; south africa; germany;</t>
-  </si>
-  <si>
     <t>usa; uk; spain; japan; canada; france; australia; india; mexico; switzerland; turkey</t>
   </si>
   <si>
-    <t>usa; canada; uk; brazil; australia; italy; china; slovakia; spain; spain; sweden; new zealand;</t>
-  </si>
-  <si>
-    <t>usa; uk; australia; india; germany; spain; canada; netherlands; new zealand; italy; signapor; argentina</t>
-  </si>
-  <si>
     <t>switzerland; usa; uk; canada; luxembourg; ireland; italy; belgium; france; australia; Denmark; norway; germany</t>
   </si>
   <si>
@@ -143,9 +122,6 @@
     <t>usa; uk; france; spain; germany; canada; iran; india; switzerland; australia; japan</t>
   </si>
   <si>
-    <t>usa; uk; canada; brazil; australia; south africa; greece; india; italy; japan; new zealand;</t>
-  </si>
-  <si>
     <t xml:space="preserve">usa; uk; australia; india; germany; spain; france; russia; china; new zealand; canada; </t>
   </si>
   <si>
@@ -161,9 +137,6 @@
     <t>usa; uk; india; australia; germany; spain; portugal; france; russia; china; italy</t>
   </si>
   <si>
-    <t>switzerland; uk; luxembourg; canada; italy; netherlands; usa; belgium; chile; south africa; sweden; uae;</t>
-  </si>
-  <si>
     <t>usa; uk; canada; france; spain; germany; switzerland; australia; india; japan; netherlands</t>
   </si>
   <si>
@@ -182,15 +155,9 @@
     <t>uk; usa; brazil; canada; italy; russia; india; serbia; australia; estonia</t>
   </si>
   <si>
-    <t>usa; uk; india; australia; germany; spain; japan; russia; new zealand; signapor; canada; france</t>
-  </si>
-  <si>
     <t>italy; switzerland; usa; luxembourg; sweden; belgium; australia; uk; canada; chile; germany; ireland; netherlands; philipines; south africa</t>
   </si>
   <si>
-    <t xml:space="preserve">usa; brazil; uk; canada; france; germany; spain; iran; australia; japan; switzerland; </t>
-  </si>
-  <si>
     <t>usa; uk; canada; portugal; india; italy; germany; australia; brazil; russia; costa rica</t>
   </si>
   <si>
@@ -230,9 +197,6 @@
     <t>usa; australia; uk; netherlands; switzerland; brazil; canada; costa rica; finland; serbia; estonia</t>
   </si>
   <si>
-    <t xml:space="preserve">usa; uk; india; australia; germany; netherlands; signapor; canada; spain; france; italy </t>
-  </si>
-  <si>
     <t>switzerland; italy; luxembourg; usa; canada; france; uae</t>
   </si>
   <si>
@@ -254,16 +218,52 @@
     <t>usa; brazil; uk; italy; australia; germany; serbia; netherlands; slovakia; spain; belgium</t>
   </si>
   <si>
-    <t xml:space="preserve">usa; uk; india; australia; germany; canada; spain; south africa; argentina; france; netherlands; </t>
-  </si>
-  <si>
     <t>italy; usa; uk; luxembourg; sweden; switzerland; germany</t>
   </si>
   <si>
-    <t>uk; usa; signapor; india; brunei; france; australia; finland; germany; hungary; iran</t>
-  </si>
-  <si>
     <t>usa; iran; uk</t>
+  </si>
+  <si>
+    <t>switzerland; usa; italy; philipines; uk; luxembourg; kenya; sweden; canada; netherlands; south africa; germany</t>
+  </si>
+  <si>
+    <t>usa; canada; uk; brazil; australia; italy; china; slovakia; spain; spain; sweden; new zealand</t>
+  </si>
+  <si>
+    <t>usa; uk; india; australia; france; bangladesh; brazil; germany; philipines; new zealand; russia; canada; israel; italy; japan; malysia; netherlands; singapor; south africa; ukraine; uae; armenia; belgium; croatia; estonia; ireland; jamaica; jordan; nepal; nigeria; portugal; sweden; switzerland; turkey</t>
+  </si>
+  <si>
+    <t>usa; uk; australia; india; germany; spain; canada; netherlands; new zealand; italy; singapor; argentina</t>
+  </si>
+  <si>
+    <t>usa; uk; india; australia; germany; spain; japan; russia; new zealand; singapor; canada; france</t>
+  </si>
+  <si>
+    <t xml:space="preserve">usa; uk; india; australia; germany; netherlands; singapor; canada; spain; france; italy </t>
+  </si>
+  <si>
+    <t>uk; usa; singapor; india; brunei; france; australia; finland; germany; hungary; iran</t>
+  </si>
+  <si>
+    <t>usa; uk; australia; italy; costa rica; germany; greece; ireland; mexico; new zealand; sweden</t>
+  </si>
+  <si>
+    <t>usa; uk; canada; brazil; italy; india; australia; spain; norway; serbia; thailand</t>
+  </si>
+  <si>
+    <t>usa; uk; australia; india; germany; spain; canada; russia; france; italy; iran</t>
+  </si>
+  <si>
+    <t>usa; uk; india; australia; germany; canada; spain; south africa; argentina; france; netherlands</t>
+  </si>
+  <si>
+    <t>switzerland; uk; luxembourg; canada; italy; netherlands; usa; belgium; chile; south africa; sweden; uae</t>
+  </si>
+  <si>
+    <t>usa; uk; canada; brazil; australia; south africa; greece; india; italy; japan; new zealand</t>
+  </si>
+  <si>
+    <t>usa; brazil; uk; canada; france; germany; spain; iran; australia; japan; switzerland</t>
   </si>
 </sst>
 </file>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.6"/>
@@ -616,13 +616,13 @@
         <v>22</v>
       </c>
       <c r="C2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
         <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.6">
@@ -630,16 +630,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.6">
@@ -647,16 +647,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.6">
@@ -664,16 +664,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.6">
@@ -681,16 +681,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.6">
@@ -698,16 +698,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.6">
@@ -715,16 +715,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.6">
@@ -732,16 +732,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.6">
@@ -749,16 +749,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.6">
@@ -766,16 +766,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.6">
@@ -783,16 +783,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E12" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.6">
@@ -800,16 +800,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.6">
@@ -817,16 +817,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.6">
@@ -834,16 +834,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="D15" t="s">
         <v>76</v>
       </c>
       <c r="E15" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.6">
@@ -851,13 +851,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="E16" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
adding the countries tables to the repository
</commit_message>
<xml_diff>
--- a/Data/countries.xlsx
+++ b/Data/countries.xlsx
@@ -122,9 +122,6 @@
     <t>usa; uk; france; spain; germany; canada; iran; india; switzerland; australia; japan</t>
   </si>
   <si>
-    <t xml:space="preserve">usa; uk; australia; india; germany; spain; france; russia; china; new zealand; canada; </t>
-  </si>
-  <si>
     <t>switzerland; italy; uk; usa; germany; luxembourg; canada; netherlands; south africa; sweden; belgium; philipines; australia; Denmark; ireland; morocco; uganda; france; kenya; norway</t>
   </si>
   <si>
@@ -264,6 +261,9 @@
   </si>
   <si>
     <t>usa; brazil; uk; canada; france; germany; spain; iran; australia; japan; switzerland</t>
+  </si>
+  <si>
+    <t>usa; uk; australia; india; germany; spain; france; russia; china; new zealand; canada</t>
   </si>
 </sst>
 </file>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.6"/>
@@ -616,10 +616,10 @@
         <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
         <v>23</v>
@@ -633,13 +633,13 @@
         <v>24</v>
       </c>
       <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" t="s">
         <v>74</v>
       </c>
-      <c r="D3" t="s">
-        <v>75</v>
-      </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.6">
@@ -650,10 +650,10 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
         <v>26</v>
@@ -684,13 +684,13 @@
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" t="s">
         <v>32</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.6">
@@ -698,16 +698,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
         <v>34</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>35</v>
       </c>
-      <c r="D7" t="s">
-        <v>36</v>
-      </c>
       <c r="E7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.6">
@@ -715,16 +715,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
         <v>37</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>38</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>39</v>
-      </c>
-      <c r="E8" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.6">
@@ -732,16 +732,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" t="s">
         <v>42</v>
-      </c>
-      <c r="D9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.6">
@@ -749,16 +749,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
         <v>44</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>45</v>
-      </c>
-      <c r="E10" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.6">
@@ -766,16 +766,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
         <v>47</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>48</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>49</v>
-      </c>
-      <c r="E11" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.6">
@@ -783,16 +783,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
         <v>51</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>52</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>53</v>
-      </c>
-      <c r="E12" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.6">
@@ -800,16 +800,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
         <v>55</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" t="s">
         <v>56</v>
-      </c>
-      <c r="D13" t="s">
-        <v>71</v>
-      </c>
-      <c r="E13" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.6">
@@ -817,16 +817,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
         <v>58</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>59</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>60</v>
-      </c>
-      <c r="E14" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.6">
@@ -834,16 +834,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
         <v>62</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" t="s">
         <v>63</v>
-      </c>
-      <c r="D15" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.6">
@@ -851,13 +851,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E16" t="s">
         <v>21</v>

</xml_diff>